<commit_message>
Build time calculator and new cycle
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235E0B9A-4A6B-4751-B14F-190FC1D65188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA7E22D-B97E-4ED3-B77E-6FBA0005EF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="195">
   <si>
     <t>Player</t>
   </si>
@@ -603,6 +603,24 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=yilIU66NTQY</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MdXiEzR1jPc</t>
+  </si>
+  <si>
+    <t>https://youtu.be/vkK-e_3bsdA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/VYkFtBW98dk</t>
+  </si>
+  <si>
+    <t>https://youtu.be/7bufkQURXws</t>
+  </si>
+  <si>
+    <t>https://youtu.be/fJEhZk7LCBs</t>
+  </si>
+  <si>
+    <t>https://youtu.be/43lz1jxkiAo</t>
   </si>
 </sst>
 </file>
@@ -659,7 +677,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -742,14 +760,21 @@
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
       <right style="medium">
         <color rgb="FFCCCCCC"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -757,9 +782,37 @@
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -767,7 +820,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -796,12 +849,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -814,7 +861,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -831,6 +878,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1147,17 +1222,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="21"/>
+    <col min="3" max="3" width="31.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="19"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.5546875" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" customWidth="1"/>
@@ -1175,7 +1250,7 @@
       <c r="B1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1745,7 +1820,7 @@
       <c r="B16" s="2">
         <v>3</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>148</v>
       </c>
       <c r="D16" s="3">
@@ -1821,7 +1896,7 @@
       <c r="B18" s="2">
         <v>4</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>131</v>
       </c>
       <c r="D18" s="3">
@@ -1859,7 +1934,7 @@
       <c r="B19" s="5">
         <v>5</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="12" t="s">
         <v>132</v>
       </c>
       <c r="D19" s="3">
@@ -1897,7 +1972,7 @@
       <c r="B20" s="5">
         <v>5</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>133</v>
       </c>
       <c r="D20" s="3">
@@ -1935,7 +2010,7 @@
       <c r="B21" s="5">
         <v>5</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="12" t="s">
         <v>134</v>
       </c>
       <c r="D21" s="3">
@@ -1973,7 +2048,7 @@
       <c r="B22" s="5">
         <v>5</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="12" t="s">
         <v>135</v>
       </c>
       <c r="D22" s="3">
@@ -2011,7 +2086,7 @@
       <c r="B23" s="5">
         <v>5</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>147</v>
       </c>
       <c r="D23" s="3">
@@ -2049,7 +2124,7 @@
       <c r="B24" s="5">
         <v>5</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="12" t="s">
         <v>136</v>
       </c>
       <c r="D24" s="3">
@@ -2087,7 +2162,7 @@
       <c r="B25" s="5">
         <v>5</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>137</v>
       </c>
       <c r="D25" s="3">
@@ -2125,7 +2200,7 @@
       <c r="B26" s="5">
         <v>5</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>148</v>
       </c>
       <c r="D26" s="3">
@@ -2163,7 +2238,7 @@
       <c r="B27" s="5">
         <v>5</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="12" t="s">
         <v>138</v>
       </c>
       <c r="D27" s="3">
@@ -2201,7 +2276,7 @@
       <c r="B28" s="5">
         <v>5</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="12" t="s">
         <v>139</v>
       </c>
       <c r="D28" s="3">
@@ -2239,7 +2314,7 @@
       <c r="B29" s="5">
         <v>5</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="12" t="s">
         <v>140</v>
       </c>
       <c r="D29" s="3">
@@ -2277,7 +2352,7 @@
       <c r="B30" s="5">
         <v>5</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="12" t="s">
         <v>141</v>
       </c>
       <c r="D30" s="3">
@@ -2315,7 +2390,7 @@
       <c r="B31" s="5">
         <v>5</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="12" t="s">
         <v>142</v>
       </c>
       <c r="D31" s="3">
@@ -2353,7 +2428,7 @@
       <c r="B32" s="5">
         <v>5</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="12" t="s">
         <v>143</v>
       </c>
       <c r="D32" s="3">
@@ -2391,7 +2466,7 @@
       <c r="B33" s="5">
         <v>5</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="12" t="s">
         <v>144</v>
       </c>
       <c r="D33" s="3">
@@ -2429,7 +2504,7 @@
       <c r="B34" s="5">
         <v>5</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="12" t="s">
         <v>145</v>
       </c>
       <c r="D34" s="3">
@@ -2467,7 +2542,7 @@
       <c r="B35" s="5">
         <v>5</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="12" t="s">
         <v>146</v>
       </c>
       <c r="D35" s="3">
@@ -3107,25 +3182,25 @@
       </c>
     </row>
     <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="28">
         <v>6</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="29">
         <v>0.19722222222222222</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" s="27" t="s">
         <v>63</v>
       </c>
       <c r="H52" s="2" t="s">
@@ -3144,26 +3219,26 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="10" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="25">
         <v>7</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="11">
+      <c r="D53" s="26">
         <v>0.1986111111111111</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="G53" s="25" t="s">
         <v>49</v>
       </c>
       <c r="H53" s="4" t="s">
@@ -3183,25 +3258,25 @@
       </c>
     </row>
     <row r="54" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="22">
         <v>7</v>
       </c>
       <c r="C54" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="23">
         <v>0.17916666666666667</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G54" s="10" t="s">
+      <c r="G54" s="22" t="s">
         <v>49</v>
       </c>
       <c r="H54" s="4" t="s">
@@ -3224,16 +3299,16 @@
       <c r="A55" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B55" s="16">
+      <c r="B55" s="14">
         <v>8</v>
       </c>
-      <c r="C55" s="18" t="s">
+      <c r="C55" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D55" s="17">
+      <c r="D55" s="15">
         <v>0.24374999999999999</v>
       </c>
-      <c r="E55" s="19" t="s">
+      <c r="E55" s="17" t="s">
         <v>96</v>
       </c>
       <c r="F55" s="4" t="s">
@@ -3262,16 +3337,16 @@
       <c r="A56" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B56" s="16">
+      <c r="B56" s="14">
         <v>8</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D56" s="17">
+      <c r="D56" s="15">
         <v>0.28263888888888888</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="E56" s="17" t="s">
         <v>110</v>
       </c>
       <c r="F56" s="4" t="s">
@@ -3300,16 +3375,16 @@
       <c r="A57" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="16">
+      <c r="B57" s="14">
         <v>8</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="D57" s="17">
+      <c r="D57" s="15">
         <v>0.25486111111111109</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="E57" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F57" s="4" t="s">
@@ -3338,16 +3413,16 @@
       <c r="A58" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B58" s="16">
+      <c r="B58" s="14">
         <v>8</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="D58" s="17">
+      <c r="D58" s="15">
         <v>0.27916666666666667</v>
       </c>
-      <c r="E58" s="19" t="s">
+      <c r="E58" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F58" s="4" t="s">
@@ -3376,16 +3451,16 @@
       <c r="A59" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="16">
+      <c r="B59" s="14">
         <v>8</v>
       </c>
       <c r="C59" t="s">
         <v>153</v>
       </c>
-      <c r="D59" s="17">
+      <c r="D59" s="15">
         <v>0.3215277777777778</v>
       </c>
-      <c r="E59" s="19" t="s">
+      <c r="E59" s="17" t="s">
         <v>86</v>
       </c>
       <c r="F59" s="4" t="s">
@@ -3414,16 +3489,16 @@
       <c r="A60" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B60" s="16">
+      <c r="B60" s="14">
         <v>8</v>
       </c>
       <c r="C60" t="s">
         <v>154</v>
       </c>
-      <c r="D60" s="17">
+      <c r="D60" s="15">
         <v>0.19513888888888889</v>
       </c>
-      <c r="E60" s="19" t="s">
+      <c r="E60" s="17" t="s">
         <v>86</v>
       </c>
       <c r="F60" s="4" t="s">
@@ -3452,16 +3527,16 @@
       <c r="A61" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B61" s="16">
+      <c r="B61" s="14">
         <v>8</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C61" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="D61" s="17">
+      <c r="D61" s="15">
         <v>0.18888888888888888</v>
       </c>
-      <c r="E61" s="19" t="s">
+      <c r="E61" s="17" t="s">
         <v>159</v>
       </c>
       <c r="F61" s="4" t="s">
@@ -3493,13 +3568,13 @@
       <c r="B62" s="5">
         <v>8</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="D62" s="17">
+      <c r="D62" s="15">
         <v>0.17083333333333331</v>
       </c>
-      <c r="E62" s="19" t="s">
+      <c r="E62" s="17" t="s">
         <v>94</v>
       </c>
       <c r="F62" s="4" t="s">
@@ -3534,10 +3609,10 @@
       <c r="C63" t="s">
         <v>166</v>
       </c>
-      <c r="D63" s="20">
+      <c r="D63" s="18">
         <v>0.15277777777777776</v>
       </c>
-      <c r="E63" s="19" t="s">
+      <c r="E63" s="17" t="s">
         <v>94</v>
       </c>
       <c r="F63" s="4" t="s">
@@ -3569,13 +3644,13 @@
       <c r="B64" s="5">
         <v>8</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C64" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D64" s="20">
+      <c r="D64" s="18">
         <v>0.24305555555555555</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E64" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F64" s="4" t="s">
@@ -3607,13 +3682,13 @@
       <c r="B65" s="5">
         <v>8</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="C65" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D65" s="20">
+      <c r="D65" s="18">
         <v>0.22222222222222221</v>
       </c>
-      <c r="E65" s="19" t="s">
+      <c r="E65" s="17" t="s">
         <v>96</v>
       </c>
       <c r="F65" s="4" t="s">
@@ -3645,13 +3720,13 @@
       <c r="B66" s="5">
         <v>8</v>
       </c>
-      <c r="C66" s="15" t="s">
+      <c r="C66" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="D66" s="20">
+      <c r="D66" s="18">
         <v>0.22083333333333333</v>
       </c>
-      <c r="E66" s="19" t="s">
+      <c r="E66" s="17" t="s">
         <v>178</v>
       </c>
       <c r="F66" s="4" t="s">
@@ -3683,13 +3758,13 @@
       <c r="B67" s="5">
         <v>8</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="C67" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="D67" s="20">
+      <c r="D67" s="18">
         <v>0.21111111111111111</v>
       </c>
-      <c r="E67" s="19" t="s">
+      <c r="E67" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F67" s="4" t="s">
@@ -3721,13 +3796,13 @@
       <c r="B68" s="5">
         <v>8</v>
       </c>
-      <c r="C68" s="15" t="s">
+      <c r="C68" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="D68" s="20">
+      <c r="D68" s="18">
         <v>0.28888888888888892</v>
       </c>
-      <c r="E68" s="19" t="s">
+      <c r="E68" s="17" t="s">
         <v>110</v>
       </c>
       <c r="F68" s="4" t="s">
@@ -3759,13 +3834,13 @@
       <c r="B69" s="5">
         <v>8</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C69" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="D69" s="20">
+      <c r="D69" s="18">
         <v>0.34097222222222223</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="E69" s="17" t="s">
         <v>67</v>
       </c>
       <c r="F69" s="4" t="s">
@@ -3797,10 +3872,10 @@
       <c r="B70" s="5">
         <v>8</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="C70" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="D70" s="20">
+      <c r="D70" s="18">
         <v>0.30486111111111108</v>
       </c>
       <c r="E70" s="4" t="s">
@@ -3835,13 +3910,13 @@
       <c r="B71" s="5">
         <v>8</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D71" s="20">
+      <c r="D71" s="18">
         <v>0.30277777777777776</v>
       </c>
-      <c r="E71" s="19" t="s">
+      <c r="E71" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F71" s="4" t="s">
@@ -3873,13 +3948,13 @@
       <c r="B72" s="5">
         <v>8</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="C72" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D72" s="20">
+      <c r="D72" s="18">
         <v>0.22847222222222222</v>
       </c>
-      <c r="E72" s="19" t="s">
+      <c r="E72" s="17" t="s">
         <v>56</v>
       </c>
       <c r="F72" s="4" t="s">
@@ -3911,13 +3986,13 @@
       <c r="B73" s="5">
         <v>8</v>
       </c>
-      <c r="C73" s="15" t="s">
+      <c r="C73" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D73" s="20">
+      <c r="D73" s="18">
         <v>0.18819444444444444</v>
       </c>
-      <c r="E73" s="19" t="s">
+      <c r="E73" s="17" t="s">
         <v>56</v>
       </c>
       <c r="F73" s="4" t="s">
@@ -3949,13 +4024,13 @@
       <c r="B74" s="5">
         <v>8</v>
       </c>
-      <c r="C74" s="15" t="s">
+      <c r="C74" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D74" s="20">
+      <c r="D74" s="18">
         <v>0.27847222222222223</v>
       </c>
-      <c r="E74" s="19" t="s">
+      <c r="E74" s="17" t="s">
         <v>27</v>
       </c>
       <c r="F74" s="4" t="s">
@@ -3987,13 +4062,13 @@
       <c r="B75" s="5">
         <v>8</v>
       </c>
-      <c r="C75" s="15" t="s">
+      <c r="C75" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="D75" s="20">
+      <c r="D75" s="18">
         <v>0.14166666666666666</v>
       </c>
-      <c r="E75" s="19" t="s">
+      <c r="E75" s="17" t="s">
         <v>27</v>
       </c>
       <c r="F75" s="4" t="s">
@@ -4025,13 +4100,13 @@
       <c r="B76" s="5">
         <v>8</v>
       </c>
-      <c r="C76" s="15" t="s">
+      <c r="C76" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="D76" s="20">
+      <c r="D76" s="18">
         <v>0.23333333333333331</v>
       </c>
-      <c r="E76" s="19" t="s">
+      <c r="E76" s="17" t="s">
         <v>86</v>
       </c>
       <c r="F76" s="4" t="s">
@@ -4063,13 +4138,13 @@
       <c r="B77" s="5">
         <v>9</v>
       </c>
-      <c r="C77" s="15" t="s">
+      <c r="C77" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="D77" s="20">
+      <c r="D77" s="18">
         <v>0.14444444444444446</v>
       </c>
-      <c r="E77" s="19" t="s">
+      <c r="E77" s="17" t="s">
         <v>159</v>
       </c>
       <c r="F77" s="4" t="s">
@@ -4101,13 +4176,13 @@
       <c r="B78" s="5">
         <v>9</v>
       </c>
-      <c r="C78" s="15" t="s">
+      <c r="C78" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="D78" s="20">
+      <c r="D78" s="18">
         <v>0.22152777777777777</v>
       </c>
-      <c r="E78" s="19" t="s">
+      <c r="E78" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F78" s="4" t="s">
@@ -4139,13 +4214,13 @@
       <c r="B79" s="5">
         <v>9</v>
       </c>
-      <c r="C79" s="15" t="s">
+      <c r="C79" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="D79" s="20">
+      <c r="D79" s="18">
         <v>0.13958333333333334</v>
       </c>
-      <c r="E79" s="19" t="s">
+      <c r="E79" s="17" t="s">
         <v>159</v>
       </c>
       <c r="F79" s="4" t="s">
@@ -4168,6 +4243,234 @@
       </c>
       <c r="L79" s="4" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B80" s="5">
+        <v>9</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D80" s="18">
+        <v>0.21597222222222223</v>
+      </c>
+      <c r="E80" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="G80" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H80" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I80" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J80" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K80" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="L80" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A81" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B81" s="5">
+        <v>9</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D81" s="18">
+        <v>0.19652777777777777</v>
+      </c>
+      <c r="E81" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F81" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G81" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H81" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I81" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J81" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="K81" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="L81" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A82" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" s="5">
+        <v>9</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D82" s="18">
+        <v>0.17847222222222223</v>
+      </c>
+      <c r="E82" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F82" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G82" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H82" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I82" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="J82" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K82" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="L82" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A83" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" s="5">
+        <v>9</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D83" s="18">
+        <v>0.30138888888888887</v>
+      </c>
+      <c r="E83" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F83" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G83" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H83" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="I83" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="J83" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K83" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L83" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A84" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B84" s="5">
+        <v>9</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D84" s="18">
+        <v>0.19513888888888889</v>
+      </c>
+      <c r="E84" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="F84" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G84" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="H84" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I84" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J84" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K84" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="L84" s="20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A85" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" s="5">
+        <v>9</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D85" s="18">
+        <v>0.21388888888888891</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F85" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G85" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H85" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I85" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J85" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="K85" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="L85" s="20" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly Update and cycle sort fix
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E078DA1B-84EA-4D10-8405-FADD30EB72CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B52058-3B6D-42C4-9FC5-525F559A38D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="202">
   <si>
     <t>Player</t>
   </si>
@@ -630,6 +630,18 @@
   </si>
   <si>
     <t>Kaeya</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=d5_vxtrOUg8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Z4hsqVwV308</t>
+  </si>
+  <si>
+    <t>https://youtu.be/VIh3RUIfBOI</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MDbqjALh8Po</t>
   </si>
 </sst>
 </file>
@@ -829,7 +841,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -910,9 +922,13 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1231,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="B76" workbookViewId="0">
+      <selection activeCell="M90" sqref="M90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4483,7 +4499,7 @@
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A86" s="28" t="s">
+      <c r="A86" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B86" s="5">
@@ -4495,29 +4511,181 @@
       <c r="D86" s="18">
         <v>0.15902777777777777</v>
       </c>
-      <c r="E86" s="29" t="s">
+      <c r="E86" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="F86" s="28" t="s">
+      <c r="F86" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G86" s="28" t="s">
+      <c r="G86" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H86" s="28" t="s">
+      <c r="H86" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="I86" s="28" t="s">
+      <c r="I86" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="J86" s="28" t="s">
+      <c r="J86" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K86" s="28" t="s">
+      <c r="K86" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L86" s="28" t="s">
+      <c r="L86" s="4" t="s">
         <v>197</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A87" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B87" s="5">
+        <v>10</v>
+      </c>
+      <c r="C87" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D87" s="18">
+        <v>0.23680555555555557</v>
+      </c>
+      <c r="E87" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="F87" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="G87" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="H87" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I87" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="J87" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="K87" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="L87" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A88" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B88" s="28">
+        <v>10</v>
+      </c>
+      <c r="C88" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="D88" s="18">
+        <v>0.19513888888888889</v>
+      </c>
+      <c r="E88" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F88" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="G88" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="H88" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="I88" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="J88" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="K88" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="L88" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A89" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B89" s="28">
+        <v>10</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D89" s="18">
+        <v>0.27569444444444446</v>
+      </c>
+      <c r="E89" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="F89" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="G89" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="H89" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I89" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J89" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="K89" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L89" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A90" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B90" s="28">
+        <v>10</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D90" s="18">
+        <v>0.20902777777777778</v>
+      </c>
+      <c r="E90" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="F90" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G90" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H90" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="I90" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J90" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="K90" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L90" s="29" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
leaderboard updated for cycle 13
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5196E8DF-C32E-49D6-82D3-DC356200D4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0D0945-1D12-480C-86D1-0C44D195C361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="221">
   <si>
     <t>Player</t>
   </si>
@@ -669,6 +669,36 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=5Yc0m8I4NTI</t>
+  </si>
+  <si>
+    <t>Kirara</t>
+  </si>
+  <si>
+    <t>Pneuma</t>
+  </si>
+  <si>
+    <t>Mika</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Uq1My9uwTVU</t>
+  </si>
+  <si>
+    <t>https://youtu.be/GHQb1hkl_SY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XUTD5azkIgQ</t>
+  </si>
+  <si>
+    <t>https://youtu.be/fD0_bAB4i-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/UYg76TbLkK0 </t>
+  </si>
+  <si>
+    <t>https://youtu.be/kFNd8W-57jU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/nK79AiNT0rI </t>
   </si>
 </sst>
 </file>
@@ -868,7 +898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -949,11 +979,10 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1274,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L98"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
-      <selection activeCell="M98" sqref="M98"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4982,41 +5011,307 @@
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A98" s="29" t="s">
+      <c r="A98" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B98" s="5">
         <v>10</v>
       </c>
-      <c r="C98" s="28" t="s">
+      <c r="C98" t="s">
         <v>210</v>
       </c>
       <c r="D98" s="18">
         <v>0.22569444444444445</v>
       </c>
-      <c r="E98" s="30" t="s">
+      <c r="E98" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F98" s="29" t="s">
+      <c r="F98" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G98" s="29" t="s">
+      <c r="G98" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H98" s="29" t="s">
+      <c r="H98" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I98" s="31" t="s">
+      <c r="I98" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J98" s="31" t="s">
+      <c r="J98" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K98" s="31" t="s">
+      <c r="K98" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L98" s="31" t="s">
+      <c r="L98" s="5" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A99" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B99" s="5">
+        <v>13</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D99" s="18">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="E99" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F99" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G99" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H99" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="I99" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J99" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K99" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L99" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A100" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" s="5">
+        <v>13</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="D100" s="18">
+        <v>0.15902777777777777</v>
+      </c>
+      <c r="E100" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F100" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G100" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H100" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="I100" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K100" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L100" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A101" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="B101" s="5">
+        <v>13</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D101" s="18">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="E101" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F101" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G101" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="H101" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I101" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J101" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="K101" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L101" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A102" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="5">
+        <v>13</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D102" s="18">
+        <v>0.19305555555555554</v>
+      </c>
+      <c r="E102" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="F102" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G102" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="H102" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="I102" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J102" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K102" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L102" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A103" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="B103" s="5">
+        <v>13</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="D103" s="18">
+        <v>0.18541666666666667</v>
+      </c>
+      <c r="E103" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F103" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="G103" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="H103" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="I103" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J103" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K103" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L103" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A104" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104" s="30">
+        <v>13</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="D104" s="18">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E104" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F104" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="G104" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="H104" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K104" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L104" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A105" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B105" s="30">
+        <v>13</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D105" s="18">
+        <v>0.17291666666666669</v>
+      </c>
+      <c r="E105" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F105" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="G105" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="H105" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I105" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J105" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K105" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="L105" s="5" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Leaderboard updated cycle 14
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0D0945-1D12-480C-86D1-0C44D195C361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1D0211-9AB0-4363-A020-10DCAA7942DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="232">
   <si>
     <t>Player</t>
   </si>
@@ -699,6 +699,39 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/nK79AiNT0rI </t>
+  </si>
+  <si>
+    <t>Juslin</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MZBcSgAIuhY</t>
+  </si>
+  <si>
+    <t>Yuenn</t>
+  </si>
+  <si>
+    <t>https://youtu.be/RFPCq2sNYm4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/XE4jSi3djzA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/HSlS5HOitO0</t>
+  </si>
+  <si>
+    <t>https://youtu.be/97ov6tiQYfA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Dsccb4tic3g</t>
+  </si>
+  <si>
+    <t>https://youtu.be/AxVCiy03OOg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/nREJpgWOAtY</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -898,7 +931,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -979,14 +1012,17 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1303,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="L113" sqref="L113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5049,7 +5085,7 @@
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99" s="29" t="s">
+      <c r="A99" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B99" s="5">
@@ -5061,16 +5097,16 @@
       <c r="D99" s="18">
         <v>0.23958333333333334</v>
       </c>
-      <c r="E99" s="28" t="s">
+      <c r="E99" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F99" s="29" t="s">
+      <c r="F99" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G99" s="29" t="s">
+      <c r="G99" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H99" s="29" t="s">
+      <c r="H99" s="4" t="s">
         <v>175</v>
       </c>
       <c r="I99" s="5" t="s">
@@ -5087,7 +5123,7 @@
       </c>
     </row>
     <row r="100" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A100" s="29" t="s">
+      <c r="A100" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B100" s="5">
@@ -5099,16 +5135,16 @@
       <c r="D100" s="18">
         <v>0.15902777777777777</v>
       </c>
-      <c r="E100" s="28" t="s">
+      <c r="E100" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F100" s="29" t="s">
+      <c r="F100" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G100" s="29" t="s">
+      <c r="G100" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H100" s="29" t="s">
+      <c r="H100" s="4" t="s">
         <v>211</v>
       </c>
       <c r="I100" s="5" t="s">
@@ -5125,7 +5161,7 @@
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A101" s="29" t="s">
+      <c r="A101" s="4" t="s">
         <v>212</v>
       </c>
       <c r="B101" s="5">
@@ -5137,16 +5173,16 @@
       <c r="D101" s="18">
         <v>5.6944444444444443E-2</v>
       </c>
-      <c r="E101" s="28" t="s">
+      <c r="E101" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F101" s="29" t="s">
+      <c r="F101" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G101" s="29" t="s">
+      <c r="G101" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H101" s="29" t="s">
+      <c r="H101" s="4" t="s">
         <v>39</v>
       </c>
       <c r="I101" s="5" t="s">
@@ -5163,7 +5199,7 @@
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A102" s="29" t="s">
+      <c r="A102" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B102" s="5">
@@ -5175,16 +5211,16 @@
       <c r="D102" s="18">
         <v>0.19305555555555554</v>
       </c>
-      <c r="E102" s="28" t="s">
+      <c r="E102" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="F102" s="29" t="s">
+      <c r="F102" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="G102" s="29" t="s">
+      <c r="G102" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H102" s="29" t="s">
+      <c r="H102" s="4" t="s">
         <v>23</v>
       </c>
       <c r="I102" s="5" t="s">
@@ -5201,7 +5237,7 @@
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A103" s="29" t="s">
+      <c r="A103" s="4" t="s">
         <v>160</v>
       </c>
       <c r="B103" s="5">
@@ -5213,16 +5249,16 @@
       <c r="D103" s="18">
         <v>0.18541666666666667</v>
       </c>
-      <c r="E103" s="28" t="s">
+      <c r="E103" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="F103" s="29" t="s">
+      <c r="F103" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G103" s="29" t="s">
+      <c r="G103" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="H103" s="29" t="s">
+      <c r="H103" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I103" s="5" t="s">
@@ -5239,10 +5275,10 @@
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A104" s="29" t="s">
+      <c r="A104" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B104" s="30">
+      <c r="B104" s="5">
         <v>13</v>
       </c>
       <c r="C104" s="13" t="s">
@@ -5251,16 +5287,16 @@
       <c r="D104" s="18">
         <v>0.29166666666666669</v>
       </c>
-      <c r="E104" s="28" t="s">
+      <c r="E104" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F104" s="29" t="s">
+      <c r="F104" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G104" s="29" t="s">
+      <c r="G104" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H104" s="29" t="s">
+      <c r="H104" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I104" s="5" t="s">
@@ -5277,10 +5313,10 @@
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A105" s="29" t="s">
+      <c r="A105" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B105" s="30">
+      <c r="B105" s="5">
         <v>13</v>
       </c>
       <c r="C105" s="13" t="s">
@@ -5289,16 +5325,16 @@
       <c r="D105" s="18">
         <v>0.17291666666666669</v>
       </c>
-      <c r="E105" s="28" t="s">
+      <c r="E105" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F105" s="29" t="s">
+      <c r="F105" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G105" s="29" t="s">
+      <c r="G105" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H105" s="29" t="s">
+      <c r="H105" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I105" s="5" t="s">
@@ -5312,6 +5348,310 @@
       </c>
       <c r="L105" s="5" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A106" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B106" s="5">
+        <v>13</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D106" s="18">
+        <v>0.16944444444444443</v>
+      </c>
+      <c r="E106" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F106" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G106" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="H106" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K106" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L106" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A107" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" s="5">
+        <v>13</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D107" s="18">
+        <v>0.28819444444444448</v>
+      </c>
+      <c r="E107" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F107" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="G107" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H107" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I107" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J107" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K107" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L107" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A108" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" s="5">
+        <v>13</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="D108" s="18">
+        <v>0.18541666666666667</v>
+      </c>
+      <c r="E108" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F108" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G108" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H108" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I108" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J108" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K108" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L108" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A109" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B109" s="5">
+        <v>14</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D109" s="18">
+        <v>0.2590277777777778</v>
+      </c>
+      <c r="E109" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F109" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="G109" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H109" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I109" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J109" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K109" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L109" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A110" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B110" s="30">
+        <v>14</v>
+      </c>
+      <c r="C110" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D110" s="18">
+        <v>0.21458333333333335</v>
+      </c>
+      <c r="E110" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F110" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="G110" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="H110" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I110" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J110" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K110" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="L110" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A111" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="B111" s="30">
+        <v>14</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D111" s="18">
+        <v>0.21527777777777779</v>
+      </c>
+      <c r="E111" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="F111" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G111" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="H111" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I111" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J111" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K111" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="L111" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A112" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B112" s="30">
+        <v>14</v>
+      </c>
+      <c r="C112" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D112" s="18">
+        <v>0.15694444444444444</v>
+      </c>
+      <c r="E112" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F112" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G112" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H112" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J112" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="K112" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L112" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A113" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B113" s="30">
+        <v>14</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D113" s="18">
+        <v>0.28680555555555554</v>
+      </c>
+      <c r="E113" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F113" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G113" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="H113" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="I113" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K113" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L113" s="5" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cycle 16 leaderboard update
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A018845-7E0D-446B-AB6D-475EECF9D7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCB2557-8C5F-4787-A1CE-313FC43DF6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
+    <workbookView xWindow="-2196" yWindow="2604" windowWidth="12960" windowHeight="7848" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="251">
   <si>
     <t>Player</t>
   </si>
@@ -738,6 +738,57 @@
   </si>
   <si>
     <t>Lynette</t>
+  </si>
+  <si>
+    <t>Minishooo</t>
+  </si>
+  <si>
+    <t>Luno</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Bkxh6Qd6pbQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=B1PcAzBC5x0&amp;ab_channel=Luno</t>
+  </si>
+  <si>
+    <t>https://youtu.be/OmDtsfl7230</t>
+  </si>
+  <si>
+    <t>https://youtu.be/gqpcjePQX8k</t>
+  </si>
+  <si>
+    <t>https://youtu.be/M_hQsU0UVes?si=vwqW0YIwrxqm1-ZH</t>
+  </si>
+  <si>
+    <t>https://youtu.be/wJodLJsT6I8</t>
+  </si>
+  <si>
+    <t>https://youtu.be/jVexaHmMpp4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=c8t-Wd2GUYk</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LyP5OlZNglM</t>
+  </si>
+  <si>
+    <t>https://youtu.be/5HUeaQcWmco</t>
+  </si>
+  <si>
+    <t>https://youtu.be/nGMrfLdKCNw</t>
+  </si>
+  <si>
+    <t>https://youtu.be/SxBny03u8Z8</t>
+  </si>
+  <si>
+    <t>Lyney</t>
+  </si>
+  <si>
+    <t>Hu Tao</t>
+  </si>
+  <si>
+    <t>Amber</t>
   </si>
 </sst>
 </file>
@@ -937,7 +988,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1021,7 +1072,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1339,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L114"/>
+  <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="I114" sqref="I114"/>
+    <sheetView tabSelected="1" topLeftCell="H120" workbookViewId="0">
+      <selection activeCell="M126" sqref="M126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5655,7 +5710,7 @@
       </c>
     </row>
     <row r="114" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A114" s="28" t="s">
+      <c r="A114" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B114" s="5">
@@ -5667,29 +5722,485 @@
       <c r="D114" s="18">
         <v>0.18958333333333333</v>
       </c>
-      <c r="E114" s="29" t="s">
+      <c r="E114" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F114" s="28" t="s">
+      <c r="F114" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G114" s="28" t="s">
+      <c r="G114" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H114" s="28" t="s">
+      <c r="H114" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="I114" s="29" t="s">
+      <c r="I114" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J114" s="28" t="s">
+      <c r="J114" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K114" s="28" t="s">
+      <c r="K114" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="L114" s="28" t="s">
+      <c r="L114" s="4" t="s">
         <v>233</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A115" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="B115" s="5">
+        <v>16</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D115" s="18">
+        <v>0.25486111111111109</v>
+      </c>
+      <c r="E115" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F115" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G115" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H115" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I115" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="J115" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K115" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="L115" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A116" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="B116" s="5">
+        <v>16</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="D116" s="18">
+        <v>0.21041666666666667</v>
+      </c>
+      <c r="E116" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="F116" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G116" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H116" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I116" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="J116" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K116" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L116" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A117" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B117" s="5">
+        <v>16</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D117" s="18">
+        <v>0.10972222222222222</v>
+      </c>
+      <c r="E117" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F117" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G117" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="H117" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I117" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="J117" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K117" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="L117" s="31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A118" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="5">
+        <v>16</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D118" s="18">
+        <v>0.17291666666666669</v>
+      </c>
+      <c r="E118" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F118" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G118" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="H118" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="I118" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="J118" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K118" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L118" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A119" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B119" s="5">
+        <v>16</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D119" s="18">
+        <v>0.1673611111111111</v>
+      </c>
+      <c r="E119" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="F119" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G119" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H119" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="I119" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="J119" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K119" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L119" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A120" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="B120" s="5">
+        <v>16</v>
+      </c>
+      <c r="C120" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="D120" s="18">
+        <v>0.21458333333333335</v>
+      </c>
+      <c r="E120" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="F120" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G120" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H120" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="I120" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="J120" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K120" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="L120" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A121" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B121" s="5">
+        <v>16</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D121" s="18">
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="E121" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="F121" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G121" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H121" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="I121" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="J121" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K121" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L121" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A122" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="B122" s="5">
+        <v>16</v>
+      </c>
+      <c r="C122" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D122" s="18">
+        <v>0.17847222222222223</v>
+      </c>
+      <c r="E122" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="F122" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G122" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H122" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="I122" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="J122" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K122" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L122" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A123" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B123" s="5">
+        <v>16</v>
+      </c>
+      <c r="C123" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="D123" s="18">
+        <v>8.4722222222222213E-2</v>
+      </c>
+      <c r="E123" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F123" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="G123" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="H123" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I123" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="J123" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K123" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L123" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A124" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B124" s="5">
+        <v>16</v>
+      </c>
+      <c r="C124" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D124" s="18">
+        <v>0.20486111111111113</v>
+      </c>
+      <c r="E124" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F124" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G124" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="H124" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="I124" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="J124" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K124" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L124" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A125" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B125" s="5">
+        <v>16</v>
+      </c>
+      <c r="C125" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="D125" s="18">
+        <v>0.16458333333333333</v>
+      </c>
+      <c r="E125" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F125" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G125" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="H125" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="I125" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="J125" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K125" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L125" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A126" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B126" s="5">
+        <v>16</v>
+      </c>
+      <c r="C126" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="D126" s="18">
+        <v>0.12222222222222223</v>
+      </c>
+      <c r="E126" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F126" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="G126" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H126" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="I126" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="J126" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="K126" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="L126" s="31" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mika and Freminet added
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCB2557-8C5F-4787-A1CE-313FC43DF6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAEF385-AF89-4B10-96A0-A9B3250E26C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2196" yWindow="2604" windowWidth="12960" windowHeight="7848" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="250">
   <si>
     <t>Player</t>
   </si>
@@ -783,9 +783,6 @@
   </si>
   <si>
     <t>Lyney</t>
-  </si>
-  <si>
-    <t>Hu Tao</t>
   </si>
   <si>
     <t>Amber</t>
@@ -988,7 +985,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1067,16 +1064,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1396,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H120" workbookViewId="0">
-      <selection activeCell="M126" sqref="M126"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5748,7 +5735,7 @@
       </c>
     </row>
     <row r="115" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A115" s="28" t="s">
+      <c r="A115" s="4" t="s">
         <v>234</v>
       </c>
       <c r="B115" s="5">
@@ -5760,33 +5747,33 @@
       <c r="D115" s="18">
         <v>0.25486111111111109</v>
       </c>
-      <c r="E115" s="30" t="s">
+      <c r="E115" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F115" s="28" t="s">
+      <c r="F115" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G115" s="28" t="s">
+      <c r="G115" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H115" s="28" t="s">
+      <c r="H115" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I115" s="31" t="s">
+      <c r="I115" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J115" s="31" t="s">
+      <c r="J115" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K115" s="31" t="s">
+      <c r="K115" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="L115" s="31" t="s">
+      <c r="L115" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A116" s="28" t="s">
+      <c r="A116" s="4" t="s">
         <v>235</v>
       </c>
       <c r="B116" s="5">
@@ -5798,33 +5785,33 @@
       <c r="D116" s="18">
         <v>0.21041666666666667</v>
       </c>
-      <c r="E116" s="30" t="s">
+      <c r="E116" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="F116" s="28" t="s">
+      <c r="F116" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G116" s="28" t="s">
+      <c r="G116" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H116" s="28" t="s">
+      <c r="H116" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I116" s="31" t="s">
+      <c r="I116" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="J116" s="31" t="s">
+      <c r="J116" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K116" s="31" t="s">
+      <c r="K116" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L116" s="31" t="s">
+      <c r="L116" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A117" s="28" t="s">
+      <c r="A117" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B117" s="5">
@@ -5836,33 +5823,33 @@
       <c r="D117" s="18">
         <v>0.10972222222222222</v>
       </c>
-      <c r="E117" s="30" t="s">
+      <c r="E117" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F117" s="28" t="s">
+      <c r="F117" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G117" s="28" t="s">
+      <c r="G117" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H117" s="28" t="s">
+      <c r="H117" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I117" s="31" t="s">
+      <c r="I117" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="J117" s="31" t="s">
+      <c r="J117" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K117" s="31" t="s">
+      <c r="K117" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L117" s="31" t="s">
+      <c r="L117" s="5" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A118" s="28" t="s">
+      <c r="A118" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B118" s="5">
@@ -5874,33 +5861,33 @@
       <c r="D118" s="18">
         <v>0.17291666666666669</v>
       </c>
-      <c r="E118" s="30" t="s">
+      <c r="E118" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F118" s="28" t="s">
+      <c r="F118" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G118" s="28" t="s">
+      <c r="G118" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H118" s="28" t="s">
+      <c r="H118" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I118" s="31" t="s">
+      <c r="I118" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="J118" s="31" t="s">
+      <c r="J118" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K118" s="31" t="s">
+      <c r="K118" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L118" s="31" t="s">
+      <c r="L118" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A119" s="28" t="s">
+      <c r="A119" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B119" s="5">
@@ -5912,33 +5899,33 @@
       <c r="D119" s="18">
         <v>0.1673611111111111</v>
       </c>
-      <c r="E119" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="F119" s="28" t="s">
+      <c r="E119" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F119" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G119" s="28" t="s">
+      <c r="G119" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H119" s="28" t="s">
+      <c r="H119" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I119" s="31" t="s">
+      <c r="I119" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J119" s="31" t="s">
+      <c r="J119" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K119" s="31" t="s">
+      <c r="K119" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L119" s="31" t="s">
+      <c r="L119" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A120" s="28" t="s">
+      <c r="A120" s="4" t="s">
         <v>234</v>
       </c>
       <c r="B120" s="5">
@@ -5950,33 +5937,33 @@
       <c r="D120" s="18">
         <v>0.21458333333333335</v>
       </c>
-      <c r="E120" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="F120" s="28" t="s">
+      <c r="E120" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F120" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G120" s="28" t="s">
+      <c r="G120" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H120" s="28" t="s">
+      <c r="H120" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I120" s="31" t="s">
+      <c r="I120" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J120" s="31" t="s">
+      <c r="J120" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K120" s="31" t="s">
+      <c r="K120" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="L120" s="31" t="s">
+      <c r="L120" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A121" s="28" t="s">
+      <c r="A121" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B121" s="5">
@@ -5988,33 +5975,33 @@
       <c r="D121" s="18">
         <v>0.15277777777777776</v>
       </c>
-      <c r="E121" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="F121" s="28" t="s">
+      <c r="E121" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F121" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G121" s="28" t="s">
+      <c r="G121" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H121" s="28" t="s">
+      <c r="H121" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I121" s="31" t="s">
+      <c r="I121" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J121" s="31" t="s">
+      <c r="J121" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K121" s="31" t="s">
+      <c r="K121" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L121" s="31" t="s">
+      <c r="L121" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A122" s="28" t="s">
+      <c r="A122" s="4" t="s">
         <v>160</v>
       </c>
       <c r="B122" s="5">
@@ -6026,71 +6013,71 @@
       <c r="D122" s="18">
         <v>0.17847222222222223</v>
       </c>
-      <c r="E122" s="30" t="s">
+      <c r="E122" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="F122" s="28" t="s">
+      <c r="F122" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G122" s="28" t="s">
+      <c r="G122" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H122" s="28" t="s">
+      <c r="H122" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="I122" s="31" t="s">
+      <c r="I122" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="J122" s="31" t="s">
+      <c r="J122" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K122" s="31" t="s">
+      <c r="K122" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L122" s="31" t="s">
+      <c r="L122" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A123" s="28" t="s">
+      <c r="A123" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B123" s="5">
         <v>16</v>
       </c>
-      <c r="C123" s="29" t="s">
+      <c r="C123" t="s">
         <v>244</v>
       </c>
       <c r="D123" s="18">
         <v>8.4722222222222213E-2</v>
       </c>
-      <c r="E123" s="30" t="s">
+      <c r="E123" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F123" s="28" t="s">
+      <c r="F123" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G123" s="28" t="s">
+      <c r="G123" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H123" s="28" t="s">
+      <c r="H123" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I123" s="31" t="s">
+      <c r="I123" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="J123" s="31" t="s">
+      <c r="J123" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K123" s="31" t="s">
+      <c r="K123" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L123" s="31" t="s">
+      <c r="L123" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A124" s="28" t="s">
+      <c r="A124" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B124" s="5">
@@ -6102,33 +6089,33 @@
       <c r="D124" s="18">
         <v>0.20486111111111113</v>
       </c>
-      <c r="E124" s="30" t="s">
+      <c r="E124" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F124" s="28" t="s">
+      <c r="F124" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G124" s="28" t="s">
+      <c r="G124" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="H124" s="28" t="s">
+      <c r="H124" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="I124" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="J124" s="31" t="s">
+      <c r="I124" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="J124" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K124" s="31" t="s">
+      <c r="K124" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L124" s="31" t="s">
+      <c r="L124" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A125" s="28" t="s">
+      <c r="A125" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B125" s="5">
@@ -6140,33 +6127,33 @@
       <c r="D125" s="18">
         <v>0.16458333333333333</v>
       </c>
-      <c r="E125" s="30" t="s">
+      <c r="E125" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="F125" s="28" t="s">
+      <c r="F125" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G125" s="28" t="s">
+      <c r="G125" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H125" s="28" t="s">
+      <c r="H125" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="I125" s="31" t="s">
+      <c r="I125" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="J125" s="31" t="s">
+      <c r="J125" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K125" s="31" t="s">
+      <c r="K125" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L125" s="31" t="s">
+      <c r="L125" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A126" s="28" t="s">
+      <c r="A126" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B126" s="5">
@@ -6178,28 +6165,28 @@
       <c r="D126" s="18">
         <v>0.12222222222222223</v>
       </c>
-      <c r="E126" s="30" t="s">
+      <c r="E126" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="F126" s="28" t="s">
+      <c r="F126" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="G126" s="28" t="s">
+      <c r="G126" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H126" s="28" t="s">
+      <c r="H126" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="I126" s="31" t="s">
+      <c r="I126" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J126" s="31" t="s">
+      <c r="J126" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K126" s="31" t="s">
+      <c r="K126" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="L126" s="31" t="s">
+      <c r="L126" s="5" t="s">
         <v>158</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cycle 17 updated + leaderboard
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAEF385-AF89-4B10-96A0-A9B3250E26C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D88251-70BD-4F4E-A5C3-39DFDFF44180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="254">
   <si>
     <t>Player</t>
   </si>
@@ -786,6 +786,18 @@
   </si>
   <si>
     <t>Amber</t>
+  </si>
+  <si>
+    <t>Staryy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eusT1uEZc3Q</t>
+  </si>
+  <si>
+    <t>https://youtu.be/QaOqW4RDlEY</t>
+  </si>
+  <si>
+    <t>TravelerGeo</t>
   </si>
 </sst>
 </file>
@@ -985,7 +997,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1064,6 +1076,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1381,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L126"/>
+  <dimension ref="A1:L128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+      <selection activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6190,6 +6208,82 @@
         <v>158</v>
       </c>
     </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A127" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="B127" s="5">
+        <v>16</v>
+      </c>
+      <c r="C127" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="D127" s="18">
+        <v>9.930555555555555E-2</v>
+      </c>
+      <c r="E127" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F127" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G127" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="H127" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="I127" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J127" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K127" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L127" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A128" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B128" s="5">
+        <v>16</v>
+      </c>
+      <c r="C128" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D128" s="18">
+        <v>0.19722222222222222</v>
+      </c>
+      <c r="E128" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="F128" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G128" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="H128" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="I128" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J128" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K128" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L128" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
leaderboard updated for cycle 18
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D88251-70BD-4F4E-A5C3-39DFDFF44180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C597F3-BE53-4E15-9EBB-2DF023DA4632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
+    <workbookView xWindow="-2484" yWindow="2436" windowWidth="12960" windowHeight="7848" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="267">
   <si>
     <t>Player</t>
   </si>
@@ -798,6 +798,45 @@
   </si>
   <si>
     <t>TravelerGeo</t>
+  </si>
+  <si>
+    <t>https://youtu.be/EnUm3o_kcDU?si=czVzhvOhmsCjIzKB</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LZKeeRT80_E&amp;ab_channel=yangi</t>
+  </si>
+  <si>
+    <t>https://youtu.be/HC28jzR18IQ</t>
+  </si>
+  <si>
+    <t>Neuvillette</t>
+  </si>
+  <si>
+    <t>Dank</t>
+  </si>
+  <si>
+    <t>Tmti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/FX-BVi8WNuI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/JXQoacbiObk?si=ptzdGCwo0cK4YVs9 </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=F1nd3Bys_h0&amp;t</t>
+  </si>
+  <si>
+    <t>https://youtu.be/kR6vUBqqxR0</t>
+  </si>
+  <si>
+    <t>https://youtu.be/mNowl4-K3Rg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Cab8A3zukNc?si=f7HnfISa55Jlg4eq</t>
+  </si>
+  <si>
+    <t>https://youtu.be/P9si_fxE0c0?si=MkdXwDLdAylllSU7</t>
   </si>
 </sst>
 </file>
@@ -997,7 +1036,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1079,6 +1118,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1399,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L128"/>
+  <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="I133" sqref="I133"/>
+    <sheetView tabSelected="1" topLeftCell="H128" workbookViewId="0">
+      <selection activeCell="M138" sqref="M138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6209,7 +6251,7 @@
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A127" s="28" t="s">
+      <c r="A127" s="4" t="s">
         <v>250</v>
       </c>
       <c r="B127" s="5">
@@ -6221,16 +6263,16 @@
       <c r="D127" s="18">
         <v>9.930555555555555E-2</v>
       </c>
-      <c r="E127" s="29" t="s">
+      <c r="E127" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="F127" s="28" t="s">
+      <c r="F127" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G127" s="28" t="s">
+      <c r="G127" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H127" s="28" t="s">
+      <c r="H127" s="4" t="s">
         <v>253</v>
       </c>
       <c r="I127" s="5" t="s">
@@ -6247,7 +6289,7 @@
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A128" s="28" t="s">
+      <c r="A128" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B128" s="5">
@@ -6259,16 +6301,16 @@
       <c r="D128" s="18">
         <v>0.19722222222222222</v>
       </c>
-      <c r="E128" s="29" t="s">
+      <c r="E128" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="F128" s="28" t="s">
+      <c r="F128" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G128" s="28" t="s">
+      <c r="G128" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H128" s="28" t="s">
+      <c r="H128" s="4" t="s">
         <v>158</v>
       </c>
       <c r="I128" s="5" t="s">
@@ -6282,6 +6324,386 @@
       </c>
       <c r="L128" s="5" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A129" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B129" s="5">
+        <v>17</v>
+      </c>
+      <c r="C129" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="D129" s="18">
+        <v>0.1875</v>
+      </c>
+      <c r="E129" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F129" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G129" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H129" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I129" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J129" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K129" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L129" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A130" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B130" s="5">
+        <v>17</v>
+      </c>
+      <c r="C130" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="D130" s="18">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="E130" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="F130" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G130" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H130" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I130" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J130" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K130" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="L130" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A131" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B131" s="29">
+        <v>17</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="D131" s="18">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E131" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F131" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G131" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H131" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I131" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J131" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K131" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="L131" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A132" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="B132" s="29">
+        <v>18</v>
+      </c>
+      <c r="C132" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D132" s="18">
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="E132" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F132" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G132" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H132" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I132" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J132" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="K132" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L132" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A133" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B133" s="29">
+        <v>18</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="D133" s="18">
+        <v>0.22291666666666665</v>
+      </c>
+      <c r="E133" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F133" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G133" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H133" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I133" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J133" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K133" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L133" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A134" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="B134" s="29">
+        <v>18</v>
+      </c>
+      <c r="C134" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D134" s="18">
+        <v>0.20416666666666669</v>
+      </c>
+      <c r="E134" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F134" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G134" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H134" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I134" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J134" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K134" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L134" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A135" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="B135" s="29">
+        <v>18</v>
+      </c>
+      <c r="C135" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D135" s="18">
+        <v>0.17569444444444446</v>
+      </c>
+      <c r="E135" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F135" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G135" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="H135" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="I135" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J135" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="K135" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L135" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A136" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B136" s="29">
+        <v>18</v>
+      </c>
+      <c r="C136" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D136" s="18">
+        <v>0.16805555555555554</v>
+      </c>
+      <c r="E136" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="F136" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="G136" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="H136" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I136" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J136" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K136" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="L136" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A137" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B137" s="29">
+        <v>18</v>
+      </c>
+      <c r="C137" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D137" s="18">
+        <v>0.20902777777777778</v>
+      </c>
+      <c r="E137" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="F137" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G137" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H137" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="I137" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J137" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K137" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="L137" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A138" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B138" s="29">
+        <v>18</v>
+      </c>
+      <c r="C138" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D138" s="18">
+        <v>8.6111111111111124E-2</v>
+      </c>
+      <c r="E138" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F138" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G138" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="H138" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="I138" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J138" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K138" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="L138" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Leaderboard update Cycle 1
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D6B2A9-EA73-413A-9114-9D387D96363E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CBCE89-742B-42B2-8C21-65E1FE588EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="285">
   <si>
     <t>Player</t>
   </si>
@@ -882,6 +882,15 @@
   </si>
   <si>
     <t>Beta 18</t>
+  </si>
+  <si>
+    <t>Not Logic</t>
+  </si>
+  <si>
+    <t>Baizhu</t>
+  </si>
+  <si>
+    <t>YunJin</t>
   </si>
 </sst>
 </file>
@@ -1463,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L138"/>
+  <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="F143" sqref="F143"/>
+    <sheetView tabSelected="1" topLeftCell="B127" workbookViewId="0">
+      <selection activeCell="K143" sqref="K143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6725,6 +6734,196 @@
         <v>93</v>
       </c>
       <c r="L138" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>250</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="D139" s="17">
+        <v>0.28055555555555556</v>
+      </c>
+      <c r="E139" t="s">
+        <v>178</v>
+      </c>
+      <c r="F139" t="s">
+        <v>29</v>
+      </c>
+      <c r="G139" t="s">
+        <v>35</v>
+      </c>
+      <c r="H139" t="s">
+        <v>46</v>
+      </c>
+      <c r="I139" t="s">
+        <v>105</v>
+      </c>
+      <c r="J139" t="s">
+        <v>106</v>
+      </c>
+      <c r="K139" t="s">
+        <v>253</v>
+      </c>
+      <c r="L139" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>282</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D140" s="17">
+        <v>0.18333333333333335</v>
+      </c>
+      <c r="E140" t="s">
+        <v>28</v>
+      </c>
+      <c r="F140" t="s">
+        <v>27</v>
+      </c>
+      <c r="G140" t="s">
+        <v>34</v>
+      </c>
+      <c r="H140" t="s">
+        <v>93</v>
+      </c>
+      <c r="I140" t="s">
+        <v>86</v>
+      </c>
+      <c r="J140" t="s">
+        <v>37</v>
+      </c>
+      <c r="K140" t="s">
+        <v>51</v>
+      </c>
+      <c r="L140" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>89</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D141" s="17">
+        <v>0.15069444444444444</v>
+      </c>
+      <c r="E141" t="s">
+        <v>24</v>
+      </c>
+      <c r="F141" t="s">
+        <v>34</v>
+      </c>
+      <c r="G141" t="s">
+        <v>93</v>
+      </c>
+      <c r="H141" t="s">
+        <v>91</v>
+      </c>
+      <c r="I141" t="s">
+        <v>92</v>
+      </c>
+      <c r="J141" t="s">
+        <v>45</v>
+      </c>
+      <c r="K141" t="s">
+        <v>185</v>
+      </c>
+      <c r="L141" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>1</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D142" s="17">
+        <v>0.15138888888888888</v>
+      </c>
+      <c r="E142" t="s">
+        <v>28</v>
+      </c>
+      <c r="F142" t="s">
+        <v>37</v>
+      </c>
+      <c r="G142" t="s">
+        <v>158</v>
+      </c>
+      <c r="H142" t="s">
+        <v>93</v>
+      </c>
+      <c r="I142" t="s">
+        <v>283</v>
+      </c>
+      <c r="J142" t="s">
+        <v>56</v>
+      </c>
+      <c r="K142" t="s">
+        <v>62</v>
+      </c>
+      <c r="L142" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>5</v>
+      </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
+      <c r="C143" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D143" s="17">
+        <v>0.24027777777777778</v>
+      </c>
+      <c r="E143" t="s">
+        <v>156</v>
+      </c>
+      <c r="F143" t="s">
+        <v>49</v>
+      </c>
+      <c r="G143" t="s">
+        <v>47</v>
+      </c>
+      <c r="H143" t="s">
+        <v>23</v>
+      </c>
+      <c r="I143" t="s">
+        <v>159</v>
+      </c>
+      <c r="J143" t="s">
+        <v>62</v>
+      </c>
+      <c r="K143" t="s">
+        <v>284</v>
+      </c>
+      <c r="L143" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cycle 2 trials updated
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643FA191-B131-4696-944A-ECE1AE2432E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B037B6E7-DCCF-4624-BF26-FE75A959BFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="293">
   <si>
     <t>Player</t>
   </si>
@@ -890,9 +890,6 @@
     <t>Baizhu</t>
   </si>
   <si>
-    <t>YunJin</t>
-  </si>
-  <si>
     <t>https://youtu.be/6DxEKdGHGF0</t>
   </si>
   <si>
@@ -906,6 +903,18 @@
   </si>
   <si>
     <t>https://youtu.be/_nnVKCxSLjQ</t>
+  </si>
+  <si>
+    <t>https://youtu.be/tSLkS8D5cGY?si=gF0Ghf4dwNfLMSBb</t>
+  </si>
+  <si>
+    <t>Hutao</t>
+  </si>
+  <si>
+    <t>https://youtu.be/fQ-0ucxzx7Y</t>
+  </si>
+  <si>
+    <t>Heizhou</t>
   </si>
 </sst>
 </file>
@@ -1487,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L143"/>
+  <dimension ref="A1:L145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B127" workbookViewId="0">
-      <selection activeCell="K148" sqref="K148"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6760,7 +6769,7 @@
         <v>1</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D139" s="17">
         <v>0.28055555555555556</v>
@@ -6798,7 +6807,7 @@
         <v>1</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D140" s="17">
         <v>0.18333333333333335</v>
@@ -6836,7 +6845,7 @@
         <v>1</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D141" s="17">
         <v>0.15069444444444444</v>
@@ -6874,7 +6883,7 @@
         <v>1</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D142" s="17">
         <v>0.15138888888888888</v>
@@ -6912,7 +6921,7 @@
         <v>1</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D143" s="17">
         <v>0.24027777777777778</v>
@@ -6936,10 +6945,86 @@
         <v>62</v>
       </c>
       <c r="K143" t="s">
-        <v>284</v>
+        <v>111</v>
       </c>
       <c r="L143" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>282</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+      <c r="C144" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="D144" s="17">
+        <v>0.14930555555555555</v>
+      </c>
+      <c r="E144" t="s">
+        <v>28</v>
+      </c>
+      <c r="F144" t="s">
+        <v>27</v>
+      </c>
+      <c r="G144" t="s">
+        <v>34</v>
+      </c>
+      <c r="H144" t="s">
+        <v>93</v>
+      </c>
+      <c r="I144" t="s">
+        <v>290</v>
+      </c>
+      <c r="J144" t="s">
+        <v>63</v>
+      </c>
+      <c r="K144" t="s">
+        <v>51</v>
+      </c>
+      <c r="L144" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+      <c r="C145" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="D145" s="17">
+        <v>0.25694444444444448</v>
+      </c>
+      <c r="E145" t="s">
+        <v>37</v>
+      </c>
+      <c r="F145" t="s">
+        <v>292</v>
+      </c>
+      <c r="G145" t="s">
+        <v>49</v>
+      </c>
+      <c r="H145" t="s">
+        <v>36</v>
+      </c>
+      <c r="I145" t="s">
+        <v>67</v>
+      </c>
+      <c r="J145" t="s">
+        <v>62</v>
+      </c>
+      <c r="K145" t="s">
+        <v>91</v>
+      </c>
+      <c r="L145" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
leadboard cycle 2 updated
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03266E55-2ECB-40E7-962C-6C3C32260017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6BA121-326C-4883-8F5B-B5DC35225BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="300">
   <si>
     <t>Player</t>
   </si>
@@ -927,6 +925,15 @@
   </si>
   <si>
     <t>Furina</t>
+  </si>
+  <si>
+    <t>https://youtu.be/c4lN8EpWApY?si=cML1iH7OONGiHSrA</t>
+  </si>
+  <si>
+    <t>tmty</t>
+  </si>
+  <si>
+    <t>https://youtu.be/wcdNh5GPRgo?si=lYENtBPqVkZpbsZD</t>
   </si>
 </sst>
 </file>
@@ -1508,10 +1515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L149"/>
+  <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="E149" sqref="E149"/>
+    <sheetView tabSelected="1" topLeftCell="B127" workbookViewId="0">
+      <selection activeCell="H153" sqref="H153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7188,6 +7195,82 @@
         <v>37</v>
       </c>
       <c r="L149" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>89</v>
+      </c>
+      <c r="B150">
+        <v>2</v>
+      </c>
+      <c r="C150" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D150" s="17">
+        <v>0.17291666666666669</v>
+      </c>
+      <c r="E150" t="s">
+        <v>24</v>
+      </c>
+      <c r="F150" t="s">
+        <v>29</v>
+      </c>
+      <c r="G150" t="s">
+        <v>38</v>
+      </c>
+      <c r="H150" t="s">
+        <v>233</v>
+      </c>
+      <c r="I150" t="s">
+        <v>92</v>
+      </c>
+      <c r="J150" t="s">
+        <v>45</v>
+      </c>
+      <c r="K150" t="s">
+        <v>213</v>
+      </c>
+      <c r="L150" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>298</v>
+      </c>
+      <c r="B151">
+        <v>2</v>
+      </c>
+      <c r="C151" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="D151" s="17">
+        <v>0.20972222222222223</v>
+      </c>
+      <c r="E151" t="s">
+        <v>110</v>
+      </c>
+      <c r="F151" t="s">
+        <v>29</v>
+      </c>
+      <c r="G151" t="s">
+        <v>296</v>
+      </c>
+      <c r="H151" t="s">
+        <v>97</v>
+      </c>
+      <c r="I151" t="s">
+        <v>28</v>
+      </c>
+      <c r="J151" t="s">
+        <v>158</v>
+      </c>
+      <c r="K151" t="s">
+        <v>34</v>
+      </c>
+      <c r="L151" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cycle 4 trials + updated leaderboard
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6BA121-326C-4883-8F5B-B5DC35225BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2930738C-24C2-4612-9604-C42A9F9E4CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="314">
   <si>
     <t>Player</t>
   </si>
@@ -930,10 +931,52 @@
     <t>https://youtu.be/c4lN8EpWApY?si=cML1iH7OONGiHSrA</t>
   </si>
   <si>
-    <t>tmty</t>
-  </si>
-  <si>
     <t>https://youtu.be/wcdNh5GPRgo?si=lYENtBPqVkZpbsZD</t>
+  </si>
+  <si>
+    <t>https://youtu.be/6mDkkMd6idE</t>
+  </si>
+  <si>
+    <t>Hutao</t>
+  </si>
+  <si>
+    <t>tTty</t>
+  </si>
+  <si>
+    <t>https://youtu.be/8SykPtYM5mg</t>
+  </si>
+  <si>
+    <t>Navia</t>
+  </si>
+  <si>
+    <t>https://youtu.be/gfOq1Wga8qU</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Wkv7RYaS-Qs</t>
+  </si>
+  <si>
+    <t>YunJin</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=z7Yig4M1Lfs</t>
+  </si>
+  <si>
+    <t>Tmty</t>
+  </si>
+  <si>
+    <t>https://youtu.be/f2hYwmHafPo</t>
+  </si>
+  <si>
+    <t>https://youtu.be/DJ2uIpoVHQw</t>
+  </si>
+  <si>
+    <t>Allhaitham</t>
+  </si>
+  <si>
+    <t>https://youtu.be/OVxZHxHTuPA?si=Q1NztQm6t4ao1U1z</t>
+  </si>
+  <si>
+    <t>https://youtu.be/NC2e3XpPf7U?si=WQr_1tWRjXtftghU</t>
   </si>
 </sst>
 </file>
@@ -1219,9 +1262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1259,7 +1302,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1365,7 +1408,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1507,7 +1550,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1515,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L151"/>
+  <dimension ref="A1:L160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B127" workbookViewId="0">
-      <selection activeCell="H153" sqref="H153"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="H166" sqref="H166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6971,8 +7014,8 @@
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>282</v>
+      <c r="A144" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -7085,8 +7128,8 @@
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>282</v>
+      <c r="A147" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B147">
         <v>2</v>
@@ -7161,8 +7204,8 @@
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>282</v>
+      <c r="A149" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B149">
         <v>2</v>
@@ -7238,13 +7281,13 @@
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B151">
         <v>2</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D151" s="17">
         <v>0.20972222222222223</v>
@@ -7272,6 +7315,348 @@
       </c>
       <c r="L151" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>2</v>
+      </c>
+      <c r="B152">
+        <v>2</v>
+      </c>
+      <c r="C152" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="D152" s="17">
+        <v>0.1986111111111111</v>
+      </c>
+      <c r="E152" t="s">
+        <v>300</v>
+      </c>
+      <c r="F152" t="s">
+        <v>63</v>
+      </c>
+      <c r="G152" t="s">
+        <v>51</v>
+      </c>
+      <c r="H152" t="s">
+        <v>31</v>
+      </c>
+      <c r="I152" t="s">
+        <v>257</v>
+      </c>
+      <c r="J152" t="s">
+        <v>296</v>
+      </c>
+      <c r="K152" t="s">
+        <v>283</v>
+      </c>
+      <c r="L152" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>234</v>
+      </c>
+      <c r="B153">
+        <v>3</v>
+      </c>
+      <c r="C153" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="D153" s="17">
+        <v>0.18263888888888888</v>
+      </c>
+      <c r="E153" t="s">
+        <v>22</v>
+      </c>
+      <c r="F153" t="s">
+        <v>51</v>
+      </c>
+      <c r="G153" t="s">
+        <v>97</v>
+      </c>
+      <c r="H153" t="s">
+        <v>46</v>
+      </c>
+      <c r="I153" t="s">
+        <v>303</v>
+      </c>
+      <c r="J153" t="s">
+        <v>296</v>
+      </c>
+      <c r="K153" t="s">
+        <v>63</v>
+      </c>
+      <c r="L153" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>11</v>
+      </c>
+      <c r="B154">
+        <v>3</v>
+      </c>
+      <c r="C154" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="D154" s="17">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="E154" t="s">
+        <v>257</v>
+      </c>
+      <c r="F154" t="s">
+        <v>296</v>
+      </c>
+      <c r="G154" t="s">
+        <v>23</v>
+      </c>
+      <c r="H154" t="s">
+        <v>196</v>
+      </c>
+      <c r="I154" t="s">
+        <v>300</v>
+      </c>
+      <c r="J154" t="s">
+        <v>63</v>
+      </c>
+      <c r="K154" t="s">
+        <v>51</v>
+      </c>
+      <c r="L154" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>250</v>
+      </c>
+      <c r="B155">
+        <v>3</v>
+      </c>
+      <c r="C155" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D155" s="17">
+        <v>0.12083333333333333</v>
+      </c>
+      <c r="E155" t="s">
+        <v>22</v>
+      </c>
+      <c r="F155" t="s">
+        <v>51</v>
+      </c>
+      <c r="G155" t="s">
+        <v>41</v>
+      </c>
+      <c r="H155" t="s">
+        <v>91</v>
+      </c>
+      <c r="I155" t="s">
+        <v>110</v>
+      </c>
+      <c r="J155" t="s">
+        <v>37</v>
+      </c>
+      <c r="K155" t="s">
+        <v>63</v>
+      </c>
+      <c r="L155" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>160</v>
+      </c>
+      <c r="B156">
+        <v>3</v>
+      </c>
+      <c r="C156" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="D156" s="17">
+        <v>0.15347222222222223</v>
+      </c>
+      <c r="E156" t="s">
+        <v>101</v>
+      </c>
+      <c r="F156" t="s">
+        <v>46</v>
+      </c>
+      <c r="G156" t="s">
+        <v>27</v>
+      </c>
+      <c r="H156" t="s">
+        <v>33</v>
+      </c>
+      <c r="I156" t="s">
+        <v>303</v>
+      </c>
+      <c r="J156" t="s">
+        <v>253</v>
+      </c>
+      <c r="K156" t="s">
+        <v>56</v>
+      </c>
+      <c r="L156" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>308</v>
+      </c>
+      <c r="B157">
+        <v>3</v>
+      </c>
+      <c r="C157" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="D157" s="17">
+        <v>0.19166666666666668</v>
+      </c>
+      <c r="E157" t="s">
+        <v>28</v>
+      </c>
+      <c r="F157" t="s">
+        <v>158</v>
+      </c>
+      <c r="G157" t="s">
+        <v>93</v>
+      </c>
+      <c r="H157" t="s">
+        <v>95</v>
+      </c>
+      <c r="I157" t="s">
+        <v>110</v>
+      </c>
+      <c r="J157" t="s">
+        <v>296</v>
+      </c>
+      <c r="K157" t="s">
+        <v>29</v>
+      </c>
+      <c r="L157" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>5</v>
+      </c>
+      <c r="B158">
+        <v>3</v>
+      </c>
+      <c r="C158" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D158" s="17">
+        <v>0.22361111111111112</v>
+      </c>
+      <c r="E158" t="s">
+        <v>257</v>
+      </c>
+      <c r="F158" t="s">
+        <v>296</v>
+      </c>
+      <c r="G158" t="s">
+        <v>23</v>
+      </c>
+      <c r="H158" t="s">
+        <v>157</v>
+      </c>
+      <c r="I158" t="s">
+        <v>311</v>
+      </c>
+      <c r="J158" t="s">
+        <v>62</v>
+      </c>
+      <c r="K158" t="s">
+        <v>56</v>
+      </c>
+      <c r="L158" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>308</v>
+      </c>
+      <c r="B159">
+        <v>3</v>
+      </c>
+      <c r="C159" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="D159" s="17">
+        <v>0.15625</v>
+      </c>
+      <c r="E159" t="s">
+        <v>47</v>
+      </c>
+      <c r="F159" t="s">
+        <v>51</v>
+      </c>
+      <c r="G159" t="s">
+        <v>49</v>
+      </c>
+      <c r="H159" t="s">
+        <v>46</v>
+      </c>
+      <c r="I159" t="s">
+        <v>110</v>
+      </c>
+      <c r="J159" t="s">
+        <v>296</v>
+      </c>
+      <c r="K159" t="s">
+        <v>29</v>
+      </c>
+      <c r="L159" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>223</v>
+      </c>
+      <c r="B160">
+        <v>3</v>
+      </c>
+      <c r="C160" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="D160" s="17">
+        <v>0.19652777777777777</v>
+      </c>
+      <c r="E160" t="s">
+        <v>22</v>
+      </c>
+      <c r="F160" t="s">
+        <v>97</v>
+      </c>
+      <c r="G160" t="s">
+        <v>46</v>
+      </c>
+      <c r="H160" t="s">
+        <v>51</v>
+      </c>
+      <c r="I160" t="s">
+        <v>110</v>
+      </c>
+      <c r="J160" t="s">
+        <v>37</v>
+      </c>
+      <c r="K160" t="s">
+        <v>63</v>
+      </c>
+      <c r="L160" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cycle 5 trials update
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deon Lee\.Net\JS\ProjectWB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2930738C-24C2-4612-9604-C42A9F9E4CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E01A77-B223-403B-8EEF-8F709383B15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1085581-6435-44B9-B82A-B6036D2595BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="315">
   <si>
     <t>Player</t>
   </si>
@@ -955,9 +954,6 @@
     <t>https://youtu.be/Wkv7RYaS-Qs</t>
   </si>
   <si>
-    <t>YunJin</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=z7Yig4M1Lfs</t>
   </si>
   <si>
@@ -970,13 +966,19 @@
     <t>https://youtu.be/DJ2uIpoVHQw</t>
   </si>
   <si>
-    <t>Allhaitham</t>
-  </si>
-  <si>
     <t>https://youtu.be/OVxZHxHTuPA?si=Q1NztQm6t4ao1U1z</t>
   </si>
   <si>
     <t>https://youtu.be/NC2e3XpPf7U?si=WQr_1tWRjXtftghU</t>
+  </si>
+  <si>
+    <t>https://youtu.be/puNezV-VkGY</t>
+  </si>
+  <si>
+    <t>Chevreuse</t>
+  </si>
+  <si>
+    <t>https://youtu.be/aUeKuJ6YZlY?si=Yk5_5f8G95s80jJW</t>
   </si>
 </sst>
 </file>
@@ -1558,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD59B03-84C8-48EE-AEDC-8E29E497FACA}">
-  <dimension ref="A1:L160"/>
+  <dimension ref="A1:L162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="H166" sqref="H166"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C164" sqref="C164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1569,14 +1571,14 @@
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.33203125" style="12" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="18"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.21875" customWidth="1"/>
-    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" style="18" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" style="18" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" style="18" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" style="18" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" style="18" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6836,28 +6838,28 @@
       <c r="D139" s="17">
         <v>0.28055555555555556</v>
       </c>
-      <c r="E139" t="s">
+      <c r="E139" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="F139" t="s">
+      <c r="F139" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G139" t="s">
+      <c r="G139" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H139" t="s">
+      <c r="H139" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="I139" t="s">
+      <c r="I139" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="J139" t="s">
+      <c r="J139" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="K139" t="s">
+      <c r="K139" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="L139" t="s">
+      <c r="L139" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -6874,28 +6876,28 @@
       <c r="D140" s="17">
         <v>0.18333333333333335</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F140" t="s">
+      <c r="F140" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G140" t="s">
+      <c r="G140" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H140" t="s">
+      <c r="H140" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="I140" t="s">
+      <c r="I140" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J140" t="s">
+      <c r="J140" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K140" t="s">
+      <c r="K140" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="L140" t="s">
+      <c r="L140" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -6912,28 +6914,28 @@
       <c r="D141" s="17">
         <v>0.15069444444444444</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E141" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F141" t="s">
+      <c r="F141" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G141" t="s">
+      <c r="G141" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="H141" t="s">
+      <c r="H141" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="I141" t="s">
+      <c r="I141" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="J141" t="s">
+      <c r="J141" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K141" t="s">
+      <c r="K141" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="L141" t="s">
+      <c r="L141" s="18" t="s">
         <v>213</v>
       </c>
     </row>
@@ -6950,28 +6952,28 @@
       <c r="D142" s="17">
         <v>0.15138888888888888</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E142" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F142" t="s">
+      <c r="F142" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G142" t="s">
+      <c r="G142" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="H142" t="s">
+      <c r="H142" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="I142" t="s">
+      <c r="I142" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="J142" t="s">
+      <c r="J142" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="K142" t="s">
+      <c r="K142" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="L142" t="s">
+      <c r="L142" s="18" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6988,28 +6990,28 @@
       <c r="D143" s="17">
         <v>0.24027777777777778</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="F143" t="s">
+      <c r="F143" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="G143" t="s">
+      <c r="G143" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H143" t="s">
+      <c r="H143" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I143" t="s">
+      <c r="I143" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="J143" t="s">
+      <c r="J143" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="K143" t="s">
+      <c r="K143" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="L143" t="s">
+      <c r="L143" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7026,28 +7028,28 @@
       <c r="D144" s="17">
         <v>0.14930555555555555</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E144" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F144" t="s">
+      <c r="F144" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G144" t="s">
+      <c r="G144" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H144" t="s">
+      <c r="H144" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="I144" t="s">
+      <c r="I144" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J144" t="s">
+      <c r="J144" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="K144" t="s">
+      <c r="K144" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="L144" t="s">
+      <c r="L144" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7064,28 +7066,28 @@
       <c r="D145" s="17">
         <v>0.25694444444444448</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E145" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F145" t="s">
+      <c r="F145" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G145" t="s">
+      <c r="G145" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H145" t="s">
+      <c r="H145" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I145" t="s">
+      <c r="I145" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="J145" t="s">
+      <c r="J145" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="K145" t="s">
+      <c r="K145" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="L145" t="s">
+      <c r="L145" s="18" t="s">
         <v>158</v>
       </c>
     </row>
@@ -7102,28 +7104,28 @@
       <c r="D146" s="17">
         <v>0.26944444444444443</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E146" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F146" t="s">
+      <c r="F146" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G146" t="s">
+      <c r="G146" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="H146" t="s">
+      <c r="H146" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="I146" t="s">
+      <c r="I146" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="J146" t="s">
+      <c r="J146" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="K146" t="s">
+      <c r="K146" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="L146" t="s">
+      <c r="L146" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7140,28 +7142,28 @@
       <c r="D147" s="17">
         <v>0.17291666666666669</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E147" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F147" t="s">
+      <c r="F147" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="G147" t="s">
+      <c r="G147" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H147" t="s">
+      <c r="H147" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I147" t="s">
+      <c r="I147" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J147" t="s">
+      <c r="J147" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="K147" t="s">
+      <c r="K147" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="L147" t="s">
+      <c r="L147" s="18" t="s">
         <v>93</v>
       </c>
     </row>
@@ -7178,28 +7180,28 @@
       <c r="D148" s="17">
         <v>0.18958333333333333</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E148" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F148" t="s">
+      <c r="F148" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G148" t="s">
+      <c r="G148" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H148" t="s">
+      <c r="H148" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I148" t="s">
+      <c r="I148" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J148" t="s">
+      <c r="J148" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="K148" t="s">
+      <c r="K148" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="L148" t="s">
+      <c r="L148" s="18" t="s">
         <v>283</v>
       </c>
     </row>
@@ -7216,28 +7218,28 @@
       <c r="D149" s="17">
         <v>0.16458333333333333</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E149" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F149" t="s">
+      <c r="F149" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="G149" t="s">
+      <c r="G149" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H149" t="s">
+      <c r="H149" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I149" t="s">
+      <c r="I149" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J149" t="s">
+      <c r="J149" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="K149" t="s">
+      <c r="K149" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="L149" t="s">
+      <c r="L149" s="18" t="s">
         <v>93</v>
       </c>
     </row>
@@ -7254,28 +7256,28 @@
       <c r="D150" s="17">
         <v>0.17291666666666669</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E150" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F150" t="s">
+      <c r="F150" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G150" t="s">
+      <c r="G150" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H150" t="s">
+      <c r="H150" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="I150" t="s">
+      <c r="I150" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="J150" t="s">
+      <c r="J150" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K150" t="s">
+      <c r="K150" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="L150" t="s">
+      <c r="L150" s="18" t="s">
         <v>185</v>
       </c>
     </row>
@@ -7292,28 +7294,28 @@
       <c r="D151" s="17">
         <v>0.20972222222222223</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E151" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="F151" t="s">
+      <c r="F151" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G151" t="s">
+      <c r="G151" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="H151" t="s">
+      <c r="H151" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="I151" t="s">
+      <c r="I151" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J151" t="s">
+      <c r="J151" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="K151" t="s">
+      <c r="K151" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="L151" t="s">
+      <c r="L151" s="18" t="s">
         <v>93</v>
       </c>
     </row>
@@ -7330,28 +7332,28 @@
       <c r="D152" s="17">
         <v>0.1986111111111111</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E152" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="F152" t="s">
+      <c r="F152" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="G152" t="s">
+      <c r="G152" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H152" t="s">
+      <c r="H152" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I152" t="s">
+      <c r="I152" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="J152" t="s">
+      <c r="J152" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="K152" t="s">
+      <c r="K152" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="L152" t="s">
+      <c r="L152" s="18" t="s">
         <v>196</v>
       </c>
     </row>
@@ -7368,28 +7370,28 @@
       <c r="D153" s="17">
         <v>0.18263888888888888</v>
       </c>
-      <c r="E153" t="s">
+      <c r="E153" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F153" t="s">
+      <c r="F153" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G153" t="s">
+      <c r="G153" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="H153" t="s">
+      <c r="H153" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="I153" t="s">
+      <c r="I153" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="J153" t="s">
+      <c r="J153" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="K153" t="s">
+      <c r="K153" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="L153" t="s">
+      <c r="L153" s="18" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7406,28 +7408,28 @@
       <c r="D154" s="17">
         <v>0.13541666666666666</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E154" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="F154" t="s">
+      <c r="F154" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="G154" t="s">
+      <c r="G154" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H154" t="s">
+      <c r="H154" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="I154" t="s">
+      <c r="I154" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="J154" t="s">
+      <c r="J154" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="K154" t="s">
+      <c r="K154" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="L154" t="s">
+      <c r="L154" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7444,29 +7446,29 @@
       <c r="D155" s="17">
         <v>0.12083333333333333</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E155" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F155" t="s">
+      <c r="F155" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G155" t="s">
+      <c r="G155" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="H155" t="s">
+      <c r="H155" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="I155" t="s">
+      <c r="I155" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="J155" t="s">
+      <c r="J155" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K155" t="s">
+      <c r="K155" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="L155" t="s">
-        <v>306</v>
+      <c r="L155" s="18" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.3">
@@ -7477,71 +7479,71 @@
         <v>3</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D156" s="17">
         <v>0.15347222222222223</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E156" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="F156" t="s">
+      <c r="F156" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G156" t="s">
+      <c r="G156" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H156" t="s">
+      <c r="H156" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I156" t="s">
+      <c r="I156" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="J156" t="s">
+      <c r="J156" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="K156" t="s">
+      <c r="K156" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="L156" t="s">
+      <c r="L156" s="18" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B157">
         <v>3</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D157" s="17">
         <v>0.19166666666666668</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E157" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F157" t="s">
+      <c r="F157" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="G157" t="s">
+      <c r="G157" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="H157" t="s">
+      <c r="H157" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="I157" t="s">
+      <c r="I157" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="J157" t="s">
+      <c r="J157" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="K157" t="s">
+      <c r="K157" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="L157" t="s">
+      <c r="L157" s="18" t="s">
         <v>97</v>
       </c>
     </row>
@@ -7553,71 +7555,71 @@
         <v>3</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D158" s="17">
         <v>0.22361111111111112</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E158" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="F158" t="s">
+      <c r="F158" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="G158" t="s">
+      <c r="G158" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H158" t="s">
+      <c r="H158" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="I158" t="s">
-        <v>311</v>
-      </c>
-      <c r="J158" t="s">
+      <c r="I158" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="J158" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="K158" t="s">
+      <c r="K158" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="L158" t="s">
+      <c r="L158" s="18" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B159">
         <v>3</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D159" s="17">
         <v>0.15625</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E159" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F159" t="s">
+      <c r="F159" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G159" t="s">
+      <c r="G159" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H159" t="s">
+      <c r="H159" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="I159" t="s">
+      <c r="I159" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="J159" t="s">
+      <c r="J159" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="K159" t="s">
+      <c r="K159" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="L159" t="s">
+      <c r="L159" s="18" t="s">
         <v>97</v>
       </c>
     </row>
@@ -7629,34 +7631,110 @@
         <v>3</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D160" s="17">
         <v>0.19652777777777777</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E160" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F160" t="s">
+      <c r="F160" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G160" t="s">
+      <c r="G160" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="H160" t="s">
+      <c r="H160" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="I160" t="s">
+      <c r="I160" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="J160" t="s">
+      <c r="J160" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K160" t="s">
+      <c r="K160" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="L160" t="s">
-        <v>306</v>
+      <c r="L160" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>89</v>
+      </c>
+      <c r="B161">
+        <v>4</v>
+      </c>
+      <c r="C161" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="D161" s="17">
+        <v>0.12291666666666666</v>
+      </c>
+      <c r="E161" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F161" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G161" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H161" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="I161" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J161" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K161" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="L161" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>282</v>
+      </c>
+      <c r="B162">
+        <v>4</v>
+      </c>
+      <c r="C162" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D162" s="17">
+        <v>0.11597222222222223</v>
+      </c>
+      <c r="E162" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="F162" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="G162" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H162" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="I162" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="J162" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K162" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="L162" s="18" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>